<commit_message>
Segregando acionamentos de Inbound e Outbound
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/ACTYON/MAPEAMENTO_ACTYON.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/ACTYON/MAPEAMENTO_ACTYON.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\ACTYON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40FD9F72-58B1-44BF-8C18-A6392344C8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D274548-8998-4445-87B1-26F7B6BB5B04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="787" firstSheet="3" activeTab="3" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="482">
   <si>
     <t>CPF</t>
   </si>
@@ -1476,6 +1476,27 @@
   </si>
   <si>
     <t>DATA_ACIONAMENTO_FIM</t>
+  </si>
+  <si>
+    <t>ID_SUB_AC</t>
+  </si>
+  <si>
+    <t>NOME_SUB_AC</t>
+  </si>
+  <si>
+    <t>CODIGO DO SUB ACIONAMENTO CADASTRADO</t>
+  </si>
+  <si>
+    <t>NOME DO SUB ACIONAMENTO CADASTRADO</t>
+  </si>
+  <si>
+    <t>tbsituacao_cobranca</t>
+  </si>
+  <si>
+    <t>SITUACAO_ID</t>
+  </si>
+  <si>
+    <t>tbdevedor_acionamento.SITUACAO_ID_AUX cruzando com o tbsituacao_cobranca.SITUACAO_ID</t>
   </si>
 </sst>
 </file>
@@ -7502,10 +7523,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDC3FDF-6F9A-4848-AD13-8B6EB024C104}">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="22.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -7513,8 +7534,8 @@
     <col min="1" max="1" width="22.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.44140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -7528,19 +7549,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="29" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="29" t="s">
         <v>190</v>
       </c>
       <c r="F1" s="29" t="s">
@@ -7572,15 +7593,17 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="D2" s="1">
+      <c r="C2" s="37"/>
+      <c r="D2" s="37">
         <v>10</v>
       </c>
+      <c r="E2" s="37"/>
       <c r="F2" s="37" t="s">
         <v>89</v>
       </c>
@@ -7606,15 +7629,17 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="D3" s="1">
+      <c r="C3" s="37"/>
+      <c r="D3" s="37">
         <v>50</v>
       </c>
+      <c r="E3" s="37"/>
       <c r="F3" s="37"/>
       <c r="G3" s="37"/>
       <c r="H3" s="37"/>
@@ -7626,15 +7651,17 @@
       <c r="N3" s="37"/>
     </row>
     <row r="4" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="1">
+      <c r="C4" s="37"/>
+      <c r="D4" s="37">
         <v>50</v>
       </c>
+      <c r="E4" s="37"/>
       <c r="F4" s="37"/>
       <c r="G4" s="37"/>
       <c r="H4" s="37"/>
@@ -7646,15 +7673,17 @@
       <c r="N4" s="37"/>
     </row>
     <row r="5" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="1">
+      <c r="C5" s="37"/>
+      <c r="D5" s="37">
         <v>8</v>
       </c>
+      <c r="E5" s="37"/>
       <c r="F5" s="37"/>
       <c r="G5" s="37"/>
       <c r="H5" s="37"/>
@@ -7666,15 +7695,17 @@
       <c r="N5" s="37"/>
     </row>
     <row r="6" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="37" t="s">
         <v>193</v>
       </c>
-      <c r="D6" s="1">
+      <c r="C6" s="37"/>
+      <c r="D6" s="37">
         <v>8</v>
       </c>
+      <c r="E6" s="37"/>
       <c r="F6" s="37"/>
       <c r="G6" s="37"/>
       <c r="H6" s="37"/>
@@ -7686,15 +7717,17 @@
       <c r="N6" s="37"/>
     </row>
     <row r="7" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="37" t="s">
         <v>85</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="37" t="s">
         <v>463</v>
       </c>
-      <c r="D7" s="1">
+      <c r="C7" s="37"/>
+      <c r="D7" s="37">
         <v>8</v>
       </c>
+      <c r="E7" s="37"/>
       <c r="F7" s="37" t="s">
         <v>89</v>
       </c>
@@ -7716,15 +7749,17 @@
       <c r="N7" s="37"/>
     </row>
     <row r="8" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="D8" s="1">
+      <c r="C8" s="37"/>
+      <c r="D8" s="37">
         <v>20</v>
       </c>
+      <c r="E8" s="37"/>
       <c r="F8" s="37" t="s">
         <v>89</v>
       </c>
@@ -7746,15 +7781,17 @@
       <c r="N8" s="37"/>
     </row>
     <row r="9" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="37" t="s">
         <v>138</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="D9" s="1">
+      <c r="C9" s="37"/>
+      <c r="D9" s="37">
         <v>20</v>
       </c>
+      <c r="E9" s="37"/>
       <c r="F9" s="37" t="s">
         <v>89</v>
       </c>
@@ -7776,15 +7813,17 @@
       <c r="N9" s="37"/>
     </row>
     <row r="10" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="37" t="s">
         <v>139</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="37" t="s">
         <v>254</v>
       </c>
-      <c r="D10" s="1">
+      <c r="C10" s="37"/>
+      <c r="D10" s="37">
         <v>100</v>
       </c>
+      <c r="E10" s="37"/>
       <c r="F10" s="37" t="s">
         <v>89</v>
       </c>
@@ -7806,15 +7845,17 @@
       <c r="N10" s="37"/>
     </row>
     <row r="11" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="37" t="s">
         <v>227</v>
       </c>
-      <c r="D11" s="1">
+      <c r="C11" s="37"/>
+      <c r="D11" s="37">
         <v>20</v>
       </c>
+      <c r="E11" s="37"/>
       <c r="F11" s="37" t="s">
         <v>89</v>
       </c>
@@ -7836,15 +7877,17 @@
       <c r="N11" s="37"/>
     </row>
     <row r="12" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="D12" s="1">
+      <c r="C12" s="37"/>
+      <c r="D12" s="37">
         <v>50</v>
       </c>
+      <c r="E12" s="37"/>
       <c r="F12" s="37" t="s">
         <v>89</v>
       </c>
@@ -7866,15 +7909,17 @@
       <c r="N12" s="37"/>
     </row>
     <row r="13" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="1">
-        <v>8</v>
-      </c>
+      <c r="A13" s="37" t="s">
+        <v>475</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>477</v>
+      </c>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37">
+        <v>50</v>
+      </c>
+      <c r="E13" s="37"/>
       <c r="F13" s="37" t="s">
         <v>89</v>
       </c>
@@ -7885,26 +7930,30 @@
         <v>465</v>
       </c>
       <c r="I13" s="37" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="J13" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" s="37"/>
+        <v>480</v>
+      </c>
+      <c r="K13" s="37" t="s">
+        <v>481</v>
+      </c>
       <c r="L13" s="37"/>
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
     </row>
     <row r="14" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="D14" s="1">
-        <v>8</v>
-      </c>
+      <c r="A14" s="37" t="s">
+        <v>476</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>478</v>
+      </c>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37">
+        <v>50</v>
+      </c>
+      <c r="E14" s="37"/>
       <c r="F14" s="37" t="s">
         <v>89</v>
       </c>
@@ -7915,26 +7964,28 @@
         <v>465</v>
       </c>
       <c r="I14" s="37" t="s">
-        <v>466</v>
+        <v>479</v>
       </c>
       <c r="J14" s="37" t="s">
-        <v>474</v>
+        <v>37</v>
       </c>
       <c r="K14" s="37"/>
       <c r="L14" s="37"/>
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
     </row>
-    <row r="15" spans="1:14" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="1">
-        <v>11</v>
-      </c>
+    <row r="15" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37">
+        <v>8</v>
+      </c>
+      <c r="E15" s="37"/>
       <c r="F15" s="37" t="s">
         <v>89</v>
       </c>
@@ -7948,12 +7999,76 @@
         <v>466</v>
       </c>
       <c r="J15" s="37" t="s">
-        <v>468</v>
+        <v>29</v>
       </c>
       <c r="K15" s="37"/>
       <c r="L15" s="37"/>
       <c r="M15" s="37"/>
       <c r="N15" s="37"/>
+    </row>
+    <row r="16" spans="1:14" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37">
+        <v>8</v>
+      </c>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="J16" s="37" t="s">
+        <v>474</v>
+      </c>
+      <c r="K16" s="37"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+    </row>
+    <row r="17" spans="1:14" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37">
+        <v>11</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>464</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>465</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>466</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>468</v>
+      </c>
+      <c r="K17" s="37"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Update dicionário e Metadados
</commit_message>
<xml_diff>
--- a/Documentos/Mapeamento das Fontes de Dados/ACTYON/MAPEAMENTO_ACTYON.xlsx
+++ b/Documentos/Mapeamento das Fontes de Dados/ACTYON/MAPEAMENTO_ACTYON.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\int.matheus\Desktop\DW\Data-Warehouse\Documentos\Mapeamento das Fontes de Dados\ACTYON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F50079-73DF-4F93-949C-6515459DCCCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83D6F3EA-35D0-4A00-96ED-78B7DFB79091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="678" firstSheet="3" activeTab="3" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="678" firstSheet="3" activeTab="11" xr2:uid="{40AA39DE-57CF-4226-99BA-0B59FFBB7B19}"/>
   </bookViews>
   <sheets>
     <sheet name="PAINEL" sheetId="18" state="hidden" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2071" uniqueCount="527">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2079" uniqueCount="528">
   <si>
     <t>CPF</t>
   </si>
@@ -1553,9 +1553,6 @@
     <t>tbtipo_fone</t>
   </si>
   <si>
-    <t>CÓDIGO DO STATUS DO FONE</t>
-  </si>
-  <si>
     <t>0 = POSITIVO | 1 = NEGATIVO | 2 INCONSISTENTE | 5 = BLACKLIST</t>
   </si>
   <si>
@@ -1571,9 +1568,6 @@
     <t>TELEFONE CADASTRADO</t>
   </si>
   <si>
-    <t>CHAR</t>
-  </si>
-  <si>
     <t>SMALLINT</t>
   </si>
   <si>
@@ -1632,6 +1626,15 @@
   </si>
   <si>
     <t>ID DO PAGAMENTO NO DW</t>
+  </si>
+  <si>
+    <t>STATUS DO TELEFONE</t>
+  </si>
+  <si>
+    <t>tbcontratante</t>
+  </si>
+  <si>
+    <t>contratante_id</t>
   </si>
 </sst>
 </file>
@@ -2607,10 +2610,10 @@
     </row>
     <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>452</v>
@@ -2622,7 +2625,7 @@
         <v>488</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -3100,7 +3103,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22786F84-93FF-4517-94E3-F320613466BF}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3167,10 +3172,10 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>452</v>
@@ -3182,7 +3187,7 @@
         <v>488</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -3217,7 +3222,7 @@
         <v>429</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J3" s="34" t="s">
         <v>460</v>
@@ -3251,7 +3256,7 @@
         <v>429</v>
       </c>
       <c r="I4" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J4" s="34" t="s">
         <v>497</v>
@@ -3413,7 +3418,7 @@
         <v>429</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J9" s="34" t="s">
         <v>1</v>
@@ -3428,7 +3433,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>450</v>
@@ -3447,7 +3452,7 @@
         <v>429</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J10" s="34" t="s">
         <v>432</v>
@@ -3515,7 +3520,7 @@
         <v>429</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J12" s="34" t="s">
         <v>104</v>
@@ -3530,16 +3535,16 @@
         <v>11</v>
       </c>
       <c r="B13" s="34" t="s">
+        <v>525</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>450</v>
+      </c>
+      <c r="D13" s="34">
+        <v>30</v>
+      </c>
+      <c r="E13" s="34" t="s">
         <v>500</v>
-      </c>
-      <c r="C13" s="34" t="s">
-        <v>506</v>
-      </c>
-      <c r="D13" s="34">
-        <v>1</v>
-      </c>
-      <c r="E13" s="34" t="s">
-        <v>501</v>
       </c>
       <c r="F13" s="34" t="s">
         <v>86</v>
@@ -3551,7 +3556,7 @@
         <v>429</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J13" s="34" t="s">
         <v>11</v>
@@ -3584,7 +3589,7 @@
         <v>429</v>
       </c>
       <c r="I14" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J14" s="34" t="s">
         <v>491</v>
@@ -3602,13 +3607,13 @@
         <v>492</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="D15" s="34">
         <v>2</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>86</v>
@@ -3620,7 +3625,7 @@
         <v>429</v>
       </c>
       <c r="I15" s="34" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="J15" s="34" t="s">
         <v>496</v>
@@ -3685,16 +3690,15 @@
     <mergeCell ref="F2:J2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B4DB11C-9573-4893-A458-1C975F352BD2}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -3762,10 +3766,10 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>452</v>
@@ -3777,7 +3781,7 @@
         <v>488</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -3793,7 +3797,7 @@
         <v>460</v>
       </c>
       <c r="B3" s="34" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C3" s="34" t="s">
         <v>453</v>
@@ -3812,7 +3816,7 @@
         <v>429</v>
       </c>
       <c r="I3" s="34" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J3" s="34" t="s">
         <v>460</v>
@@ -3824,10 +3828,10 @@
     </row>
     <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="34" t="s">
-        <v>460</v>
+        <v>497</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>453</v>
@@ -3835,7 +3839,9 @@
       <c r="D4" s="34">
         <v>19</v>
       </c>
-      <c r="E4" s="34"/>
+      <c r="E4" s="34">
+        <v>19</v>
+      </c>
       <c r="F4" s="34" t="s">
         <v>86</v>
       </c>
@@ -3981,17 +3987,17 @@
       <c r="N8" s="34"/>
     </row>
     <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="44" t="s">
-        <v>46</v>
+      <c r="A9" s="34" t="s">
+        <v>82</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>205</v>
+        <v>427</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D9" s="34">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="E9" s="34"/>
       <c r="F9" s="34" t="s">
@@ -4004,10 +4010,10 @@
         <v>429</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>514</v>
+        <v>526</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>1</v>
+        <v>527</v>
       </c>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
@@ -4015,17 +4021,17 @@
       <c r="N9" s="34"/>
     </row>
     <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1" t="s">
-        <v>97</v>
+      <c r="A10" s="44" t="s">
+        <v>46</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>510</v>
+        <v>205</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
       <c r="D10" s="34">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="E10" s="34"/>
       <c r="F10" s="34" t="s">
@@ -4038,10 +4044,10 @@
         <v>429</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="K10" s="34"/>
       <c r="L10" s="34"/>
@@ -4050,16 +4056,16 @@
     </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>519</v>
+        <v>97</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>450</v>
       </c>
       <c r="D11" s="34">
-        <v>30</v>
+        <v>100</v>
       </c>
       <c r="E11" s="34"/>
       <c r="F11" s="34" t="s">
@@ -4072,32 +4078,30 @@
         <v>429</v>
       </c>
       <c r="I11" s="34" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="J11" s="34" t="s">
-        <v>436</v>
+        <v>97</v>
       </c>
       <c r="K11" s="34"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
     </row>
-    <row r="12" spans="1:14" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="34" t="s">
-        <v>116</v>
+    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>517</v>
       </c>
       <c r="B12" s="34" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>450</v>
       </c>
       <c r="D12" s="34">
-        <v>20</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>517</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="E12" s="34"/>
       <c r="F12" s="34" t="s">
         <v>86</v>
       </c>
@@ -4108,30 +4112,32 @@
         <v>429</v>
       </c>
       <c r="I12" s="34" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="J12" s="34" t="s">
-        <v>518</v>
+        <v>436</v>
       </c>
       <c r="K12" s="34"/>
       <c r="L12" s="34"/>
       <c r="M12" s="34"/>
       <c r="N12" s="34"/>
     </row>
-    <row r="13" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:14" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B13" s="34" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>450</v>
       </c>
       <c r="D13" s="34">
-        <v>30</v>
-      </c>
-      <c r="E13" s="34"/>
+        <v>20</v>
+      </c>
+      <c r="E13" s="34" t="s">
+        <v>515</v>
+      </c>
       <c r="F13" s="34" t="s">
         <v>86</v>
       </c>
@@ -4142,10 +4148,10 @@
         <v>429</v>
       </c>
       <c r="I13" s="34" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="J13" s="34" t="s">
-        <v>104</v>
+        <v>516</v>
       </c>
       <c r="K13" s="34"/>
       <c r="L13" s="34"/>
@@ -4154,10 +4160,10 @@
     </row>
     <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="34" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B14" s="34" t="s">
-        <v>446</v>
+        <v>509</v>
       </c>
       <c r="C14" s="34" t="s">
         <v>450</v>
@@ -4166,34 +4172,42 @@
         <v>30</v>
       </c>
       <c r="E14" s="34"/>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="G14" s="46"/>
-      <c r="H14" s="46"/>
-      <c r="I14" s="46"/>
-      <c r="J14" s="47"/>
+      <c r="G14" s="34" t="s">
+        <v>428</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>429</v>
+      </c>
+      <c r="I14" s="34" t="s">
+        <v>512</v>
+      </c>
+      <c r="J14" s="34" t="s">
+        <v>104</v>
+      </c>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>485</v>
+      <c r="A15" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>446</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D15" s="34">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="E15" s="34"/>
       <c r="F15" s="45" t="s">
-        <v>486</v>
+        <v>86</v>
       </c>
       <c r="G15" s="46"/>
       <c r="H15" s="46"/>
@@ -4204,21 +4218,47 @@
       <c r="M15" s="34"/>
       <c r="N15" s="34"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
+    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>484</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>453</v>
+      </c>
+      <c r="D16" s="34">
+        <v>19</v>
+      </c>
+      <c r="E16" s="34"/>
+      <c r="F16" s="45" t="s">
+        <v>486</v>
+      </c>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="F2:J2"/>
-    <mergeCell ref="F14:J14"/>
     <mergeCell ref="F15:J15"/>
+    <mergeCell ref="F16:J16"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -7774,7 +7814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFDC3FDF-6F9A-4848-AD13-8B6EB024C104}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:A7"/>
     </sheetView>
   </sheetViews>
@@ -7843,10 +7883,10 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>452</v>
@@ -7858,7 +7898,7 @@
         <v>488</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>
@@ -8574,10 +8614,10 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>452</v>
@@ -8589,7 +8629,7 @@
         <v>488</v>
       </c>
       <c r="F2" s="45" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G2" s="46"/>
       <c r="H2" s="46"/>

</xml_diff>